<commit_message>
updated Poland data upto 2020-05-13, Poland without slaskie
</commit_message>
<xml_diff>
--- a/data/population.xlsx
+++ b/data/population.xlsx
@@ -11,8 +11,8 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$335</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$335</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$F$335</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$1:$G$335</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!$A$1:$F$331</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$330</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Sheet1!$A$1:$F$257</definedName>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="347">
   <si>
     <t xml:space="preserve">Province/State</t>
   </si>
@@ -1069,6 +1069,12 @@
   </si>
   <si>
     <t xml:space="preserve">Sao Tome and Principe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland without slaskie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Poland without slaskie and dolnoslaskie</t>
   </si>
 </sst>
 </file>
@@ -1218,16 +1224,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G335"/>
+  <dimension ref="A1:G337"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A314" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B338" activeCellId="0" sqref="B338"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="13.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="30.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="12.37"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="23.62"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.08"/>
@@ -7585,8 +7591,26 @@
         <v>23.75</v>
       </c>
     </row>
+    <row r="336" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B336" s="0" t="s">
+        <v>345</v>
+      </c>
+      <c r="C336" s="1" t="n">
+        <f aca="false">C185-C325</f>
+        <v>33833373</v>
+      </c>
+    </row>
+    <row r="337" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B337" s="0" t="s">
+        <v>346</v>
+      </c>
+      <c r="C337" s="1" t="n">
+        <f aca="false">C185-C325-C314</f>
+        <v>30931008</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G335"/>
+  <autoFilter ref="A1:F335"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>